<commit_message>
add testcase login, signup; testsuits
</commit_message>
<xml_diff>
--- a/login.xlsx
+++ b/login.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Katalon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Katalon\Testing-Ecommerce-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380FE2AF-AA32-41F8-9521-457711108681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F93B4FB-2DC9-4AF9-917A-B52A5C024D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{540B6645-3E0A-4AE6-874C-88B6AAE12C1E}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{540B6645-3E0A-4AE6-874C-88B6AAE12C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -34,6 +35,15 @@
   </si>
   <si>
     <t>katalon1</t>
+  </si>
+  <si>
+    <t>21002777</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>katalonfail</t>
   </si>
 </sst>
 </file>
@@ -69,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,37 +398,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E4F5FB-B8E1-42EF-8E72-E465BADC3E4D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>21020799</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>123456</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC328EA1-1F9E-4733-999D-3CED2A5294B4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>